<commit_message>
Some fixes and refinement
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="85">
   <si>
     <t xml:space="preserve">J0_BT</t>
   </si>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">47u</t>
   </si>
   <si>
-    <t xml:space="preserve">T529P476M010AAE200</t>
+    <t xml:space="preserve">T58W9476M6R3C0150</t>
   </si>
   <si>
     <t xml:space="preserve">C4</t>
@@ -142,6 +142,9 @@
     <t xml:space="preserve">1MEG</t>
   </si>
   <si>
+    <t xml:space="preserve">CR0603-FX-1004ELF</t>
+  </si>
+  <si>
     <t xml:space="preserve">R3</t>
   </si>
   <si>
@@ -199,6 +202,12 @@
     <t xml:space="preserve">J0_VOL</t>
   </si>
   <si>
+    <t xml:space="preserve">100u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMCMB1A107MTRF</t>
+  </si>
+  <si>
     <t xml:space="preserve">270p</t>
   </si>
   <si>
@@ -224,6 +233,42 @@
   </si>
   <si>
     <t xml:space="preserve">ECH-U1H102JX5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1A-13-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">282834-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR0603-FX-1003ELF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR0603-FX-2002ELF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R10</t>
   </si>
   <si>
     <t xml:space="preserve">J0_BLEND</t>
@@ -245,6 +290,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -334,26 +380,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.0051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="0"/>
+      <c r="E1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -418,10 +466,7 @@
         <v>14</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>2.13</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>1.59</v>
+        <v>0.713</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,6 +542,7 @@
       <c r="B8" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="C8" s="0"/>
       <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
@@ -514,6 +560,7 @@
       <c r="B9" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="C9" s="0"/>
       <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
@@ -534,6 +581,7 @@
       <c r="B10" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="C10" s="0"/>
       <c r="E10" s="1" t="s">
         <v>32</v>
       </c>
@@ -581,27 +629,27 @@
         <v>10</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>0.165</v>
+        <v>0.137</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>0.04</v>
+        <v>0.034</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>0.137</v>
@@ -612,16 +660,16 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>0.137</v>
@@ -632,16 +680,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>0.137</v>
@@ -652,16 +700,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>0.137</v>
@@ -672,16 +720,16 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>0.137</v>
@@ -692,19 +740,19 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>3.31</v>
@@ -713,10 +761,16 @@
         <v>2.61</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0"/>
+      <c r="E19" s="0"/>
+    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>58</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C20" s="0"/>
+      <c r="E20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -749,7 +803,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>4</v>
@@ -758,13 +812,13 @@
         <v>5</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>2.13</v>
+        <v>0.686</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>1.59</v>
+        <v>0.576</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,7 +826,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>17</v>
@@ -781,7 +835,7 @@
         <v>10</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>0.439</v>
@@ -830,10 +884,7 @@
         <v>14</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>2.13</v>
-      </c>
-      <c r="H25" s="0" t="n">
-        <v>1.59</v>
+        <v>0.713</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -841,7 +892,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>17</v>
@@ -850,7 +901,7 @@
         <v>10</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>0.439</v>
@@ -861,10 +912,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>4</v>
@@ -873,7 +924,7 @@
         <v>5</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>0.508</v>
@@ -884,7 +935,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>3</v>
@@ -907,10 +958,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>17</v>
@@ -919,7 +970,7 @@
         <v>5</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>0.768</v>
@@ -928,17 +979,321 @@
         <v>0.442</v>
       </c>
     </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>0.384</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>0.259</v>
+      </c>
+    </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>54</v>
+        <v>26</v>
+      </c>
+      <c r="C31" s="0"/>
+      <c r="E31" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G31" s="0" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="0"/>
+      <c r="E32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0.713</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>0.631</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="0"/>
+      <c r="E33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0.494</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>0.199</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="0"/>
+      <c r="E34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>0.494</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>0.199</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>0.137</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>0.137</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>0.029</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>0.137</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <v>0.029</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>0.137</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>0.137</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>0.034</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>0.137</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>0.029</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>0.137</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>0.049</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>0.137</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <v>0.029</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>0.165</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="G46" s="0" t="n">
         <v>8.63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
J BT Caps to film
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -76,7 +76,7 @@
     <t xml:space="preserve">FILM</t>
   </si>
   <si>
-    <t xml:space="preserve">ECH-U1C272GX5</t>
+    <t xml:space="preserve">ECH-U1H272GX5</t>
   </si>
   <si>
     <t xml:space="preserve">C5</t>
@@ -401,14 +401,17 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="C7:H7"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -502,6 +505,9 @@
       </c>
       <c r="G5" s="0" t="n">
         <v>0.796</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.457</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Tone cap changed to female pin strip header for 0.047uF and 0.1uF
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="126">
   <si>
     <t>J0_BT</t>
   </si>
@@ -382,6 +382,21 @@
   </si>
   <si>
     <t xml:space="preserve">ECH-U1C472GX5 </t>
+  </si>
+  <si>
+    <t>C8*</t>
+  </si>
+  <si>
+    <t>0.047u</t>
+  </si>
+  <si>
+    <t>MKP2</t>
+  </si>
+  <si>
+    <t>MKS2D031001A00KA00</t>
+  </si>
+  <si>
+    <t>MKS2D024701A00JI00</t>
   </si>
 </sst>
 </file>
@@ -726,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102:H102"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -1283,133 +1298,138 @@
         <v>71</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>3</v>
+        <v>122</v>
       </c>
       <c r="D28" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="F28" t="s">
-        <v>6</v>
+        <v>125</v>
       </c>
       <c r="G28">
-        <v>0.79600000000000004</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="H28">
-        <v>0.60099999999999998</v>
+        <v>0.501</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="D29" t="s">
         <v>17</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F29" t="s">
+        <v>124</v>
+      </c>
+      <c r="G29">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="H29">
+        <v>0.19900000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>74</v>
       </c>
-      <c r="G29">
+      <c r="G30">
         <v>0.76800000000000002</v>
       </c>
-      <c r="H29">
+      <c r="H30">
         <v>0.442</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G30">
-        <v>0.38400000000000001</v>
-      </c>
-      <c r="H30">
-        <v>0.25900000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G31">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="H31">
+        <v>0.25900000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
         <v>27</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>28</v>
-      </c>
-      <c r="C31"/>
-      <c r="E31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" t="s">
-        <v>79</v>
-      </c>
-      <c r="G31">
-        <v>1.52</v>
-      </c>
-      <c r="H31">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B32" t="s">
-        <v>31</v>
       </c>
       <c r="C32"/>
       <c r="E32" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F32" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="G32">
-        <v>0.71299999999999997</v>
+        <v>1.52</v>
       </c>
       <c r="H32">
-        <v>0.63100000000000001</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C33"/>
       <c r="E33" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G33">
-        <v>0.49399999999999999</v>
+        <v>0.71299999999999997</v>
       </c>
       <c r="H33">
-        <v>0.19900000000000001</v>
+        <v>0.63100000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="C34"/>
       <c r="E34" s="1" t="s">
@@ -1426,71 +1446,69 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35"/>
+      <c r="E35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="H35">
+        <v>0.19900000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="E36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
         <v>42</v>
       </c>
-      <c r="G35">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="H35">
+      <c r="G36">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="H36">
         <v>3.4000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B36" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" t="s">
-        <v>82</v>
-      </c>
-      <c r="G36">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="H36">
-        <v>0.04</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="G37">
-        <v>0.13700000000000001</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="H37">
-        <v>2.9000000000000001E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>53</v>
@@ -1510,172 +1528,169 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="G39">
         <v>0.13700000000000001</v>
       </c>
       <c r="H39">
-        <v>1.2E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B40" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F40" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="G40">
         <v>0.13700000000000001</v>
       </c>
       <c r="H40">
-        <v>3.4000000000000002E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="G41">
         <v>0.13700000000000001</v>
       </c>
       <c r="H41">
-        <v>2.9000000000000001E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>51</v>
+      <c r="F42" t="s">
+        <v>83</v>
       </c>
       <c r="G42">
         <v>0.13700000000000001</v>
       </c>
       <c r="H42">
-        <v>4.9000000000000002E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F43" t="s">
-        <v>57</v>
+      <c r="F43" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="G43">
         <v>0.13700000000000001</v>
       </c>
       <c r="H43">
-        <v>2.9000000000000001E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B44" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" t="s">
+        <v>57</v>
+      </c>
+      <c r="G44">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="H44">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B45" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="E45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s">
         <v>39</v>
       </c>
-      <c r="G44">
+      <c r="G45">
         <v>0.16500000000000001</v>
       </c>
-      <c r="H44">
+      <c r="H45">
         <v>0.04</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
         <v>87</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>59</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F47" t="s">
         <v>88</v>
       </c>
-      <c r="G46">
+      <c r="G47">
         <v>8.6300000000000008</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
         <v>1</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>2</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D49" t="s">
-        <v>4</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F49" t="s">
-        <v>70</v>
-      </c>
-      <c r="G49">
-        <v>0.50800000000000001</v>
-      </c>
-      <c r="H49">
-        <v>0.44600000000000001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B50" t="s">
-        <v>7</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>69</v>
@@ -1698,211 +1713,214 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B51" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="D51" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F51" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="G51">
-        <v>0.86399999999999999</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="H51">
-        <v>0.49099999999999999</v>
+        <v>0.44600000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B52" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="D52" t="s">
         <v>17</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F52" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="G52">
-        <v>0.439</v>
+        <v>0.86399999999999999</v>
       </c>
       <c r="H52">
-        <v>0.214</v>
+        <v>0.49099999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="D53" t="s">
         <v>17</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F53" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="G53">
-        <v>1.1499999999999999</v>
+        <v>0.439</v>
       </c>
       <c r="H53">
-        <v>0.66</v>
+        <v>0.214</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B54" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="D54" t="s">
         <v>17</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F54" t="s">
+        <v>91</v>
+      </c>
+      <c r="G54">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H54">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B55" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" t="s">
         <v>67</v>
       </c>
-      <c r="G54">
+      <c r="G55">
         <v>0.439</v>
       </c>
-      <c r="H54">
+      <c r="H55">
         <v>0.214</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
         <v>36</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>37</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="E56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" t="s">
         <v>57</v>
       </c>
-      <c r="G55">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="H55">
+      <c r="G56">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="H56">
         <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B56" t="s">
-        <v>40</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F56" t="s">
-        <v>116</v>
-      </c>
-      <c r="G56">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="H56">
-        <v>1.2E-2</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F57" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="G57">
         <v>0.13700000000000001</v>
       </c>
       <c r="H57">
-        <v>2.9000000000000001E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F58" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="G58">
         <v>0.13700000000000001</v>
       </c>
       <c r="H58">
-        <v>1.2E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F59" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="G59">
         <v>0.13700000000000001</v>
       </c>
       <c r="H59">
-        <v>2.9000000000000001E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B60" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F60" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="G60">
         <v>0.13700000000000001</v>
@@ -1913,7 +1931,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B61" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>60</v>
@@ -1933,78 +1951,75 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B62" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" t="s">
+        <v>83</v>
+      </c>
+      <c r="G62">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="H62">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B63" t="s">
         <v>84</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62" s="2" t="s">
+      <c r="E63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G62">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="H62">
+      <c r="G63">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="H63">
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A63" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
         <v>95</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>96</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F64" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G63">
+      <c r="G64">
         <v>1.02</v>
       </c>
-      <c r="H63">
+      <c r="H64">
         <v>0.83599999999999997</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A65" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A67" t="s">
         <v>1</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>2</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D66" t="s">
-        <v>17</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F66" t="s">
-        <v>91</v>
-      </c>
-      <c r="G66">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="H66">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B67" t="s">
-        <v>7</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>3</v>
@@ -2027,27 +2042,30 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F68" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="G68">
-        <v>0.37</v>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H68">
+        <v>0.66</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B69" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>20</v>
@@ -2061,13 +2079,16 @@
       <c r="F69" t="s">
         <v>100</v>
       </c>
+      <c r="G69">
+        <v>0.37</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="D70" t="s">
         <v>4</v>
@@ -2076,98 +2097,97 @@
         <v>5</v>
       </c>
       <c r="F70" t="s">
-        <v>70</v>
-      </c>
-      <c r="G70">
-        <v>0.50800000000000001</v>
-      </c>
-      <c r="H70">
-        <v>0.44600000000000001</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F71" t="s">
+        <v>70</v>
+      </c>
+      <c r="G71">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="H71">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B72" t="s">
         <v>23</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D72" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="E72" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" t="s">
         <v>67</v>
       </c>
-      <c r="G71">
+      <c r="G72">
         <v>0.439</v>
       </c>
-      <c r="H71">
+      <c r="H72">
         <v>0.214</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A72" t="s">
-        <v>75</v>
-      </c>
-      <c r="B72" t="s">
-        <v>76</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G72">
-        <v>0.38400000000000001</v>
-      </c>
-      <c r="H72">
-        <v>0.25900000000000001</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G73">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="H73">
+        <v>0.25900000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A74" t="s">
         <v>27</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>28</v>
-      </c>
-      <c r="C73"/>
-      <c r="E73" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F73" t="s">
-        <v>79</v>
-      </c>
-      <c r="G73">
-        <v>1.52</v>
-      </c>
-      <c r="H73">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B74" t="s">
-        <v>31</v>
       </c>
       <c r="C74"/>
       <c r="E74" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F74" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="G74">
-        <v>0.71299999999999997</v>
+        <v>1.52</v>
       </c>
       <c r="H74">
-        <v>0.63100000000000001</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.4">
@@ -2207,29 +2227,29 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A77" t="s">
-        <v>32</v>
-      </c>
       <c r="B77" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C77"/>
       <c r="E77" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F77" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G77">
-        <v>0.49399999999999999</v>
+        <v>0.71299999999999997</v>
       </c>
       <c r="H77">
-        <v>0.19900000000000001</v>
+        <v>0.63100000000000001</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A78" t="s">
+        <v>32</v>
+      </c>
       <c r="B78" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="C78"/>
       <c r="E78" s="1" t="s">
@@ -2246,31 +2266,29 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A79" t="s">
+      <c r="B79" t="s">
+        <v>80</v>
+      </c>
+      <c r="C79"/>
+      <c r="E79" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F79" t="s">
+        <v>35</v>
+      </c>
+      <c r="G79">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="H79">
+        <v>0.19900000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A80" t="s">
         <v>36</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>37</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F79" t="s">
-        <v>111</v>
-      </c>
-      <c r="G79">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="H79">
-        <v>3.4000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B80" t="s">
-        <v>40</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>108</v>
@@ -2288,18 +2306,18 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F81" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="G81">
         <v>0.13700000000000001</v>
@@ -2308,9 +2326,9 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B82" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>41</v>
@@ -2328,29 +2346,29 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B83" t="s">
+        <v>46</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" t="s">
+        <v>42</v>
+      </c>
+      <c r="G83">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="H83">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B84" t="s">
         <v>49</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F83" t="s">
-        <v>116</v>
-      </c>
-      <c r="G83">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="H83">
-        <v>3.5999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B84" t="s">
-        <v>52</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>117</v>
@@ -2368,29 +2386,29 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B85" t="s">
+        <v>52</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85" t="s">
+        <v>116</v>
+      </c>
+      <c r="G85">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="H85">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B86" t="s">
         <v>55</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F85" t="s">
-        <v>113</v>
-      </c>
-      <c r="G85">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="H85">
-        <v>3.4000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B86" t="s">
-        <v>84</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>81</v>
@@ -2408,38 +2426,38 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B87" t="s">
+        <v>84</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F87" t="s">
+        <v>113</v>
+      </c>
+      <c r="G87">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="H87">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B88" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E87" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F87" s="2" t="s">
+      <c r="E88" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="G87">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="H87">
-        <v>4.9000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B88" t="s">
-        <v>86</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="G88">
         <v>0.13700000000000001</v>
@@ -2448,38 +2466,38 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B89" t="s">
+        <v>86</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G89">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="H89">
+        <v>4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B90" t="s">
         <v>101</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E89" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="E90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F90" t="s">
         <v>54</v>
-      </c>
-      <c r="G89">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="H89">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B90" t="s">
-        <v>102</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F90" t="s">
-        <v>114</v>
       </c>
       <c r="G90">
         <v>0.13700000000000001</v>
@@ -2488,18 +2506,18 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B91" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F91" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="G91">
         <v>0.13700000000000001</v>
@@ -2508,9 +2526,9 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B92" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>60</v>
@@ -2528,18 +2546,18 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B93" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F93" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G93">
         <v>0.13700000000000001</v>
@@ -2548,9 +2566,9 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B94" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>93</v>
@@ -2568,18 +2586,18 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B95" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F95" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="G95">
         <v>0.13700000000000001</v>
@@ -2588,63 +2606,60 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A96" t="s">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B96" t="s">
+        <v>107</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F96" t="s">
+        <v>54</v>
+      </c>
+      <c r="G96">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="H96">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A97" t="s">
         <v>95</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>96</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F96" s="1" t="s">
+      <c r="F97" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G96">
+      <c r="G97">
         <v>1.02</v>
       </c>
-      <c r="H96">
+      <c r="H97">
         <v>0.83599999999999997</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A98" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A100" t="s">
         <v>1</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>2</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D99" t="s">
-        <v>17</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F99" t="s">
-        <v>92</v>
-      </c>
-      <c r="G99">
-        <v>0.86399999999999999</v>
-      </c>
-      <c r="H99">
-        <v>0.49099999999999999</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B100" t="s">
-        <v>7</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="D100" t="s">
         <v>17</v>
@@ -2652,42 +2667,45 @@
       <c r="E100" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F100" s="3" t="s">
+      <c r="F100" t="s">
+        <v>92</v>
+      </c>
+      <c r="G100">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="H100">
+        <v>0.49099999999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D101" t="s">
+        <v>17</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F101" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G100">
+      <c r="G101">
         <v>0.82299999999999995</v>
       </c>
-      <c r="H100">
+      <c r="H101">
         <v>0.47199999999999998</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A101" t="s">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A102" t="s">
         <v>36</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>37</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F101" t="s">
-        <v>114</v>
-      </c>
-      <c r="G101">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="H101">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B102" t="s">
-        <v>40</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>110</v>
@@ -2702,6 +2720,26 @@
         <v>0.13700000000000001</v>
       </c>
       <c r="H102">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B103" t="s">
+        <v>40</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F103" t="s">
+        <v>114</v>
+      </c>
+      <c r="G103">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="H103">
         <v>2.9000000000000001E-2</v>
       </c>
     </row>

</xml_diff>